<commit_message>
update data with resort sheetname
</commit_message>
<xml_diff>
--- a/数据整理/stocks/A股/上证主板/600006-东风汽车.xlsx
+++ b/数据整理/stocks/A股/上证主板/600006-东风汽车.xlsx
@@ -6,8 +6,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="总计" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="总计" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,6 +451,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>持有数量(只)</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>持有市值(亿元)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2020-Q4</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -613,56 +665,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>日期</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>持有数量(只)</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>持有市值(亿元)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2020-Q4</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>